<commit_message>
Add exercise 5 and mini project 1
</commit_message>
<xml_diff>
--- a/files/projects/01-mini-project_rubric.xlsx
+++ b/files/projects/01-mini-project_rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Sites/courses/datavizs25/files/projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Sites/courses/datavizf25/files/projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B09871F-B7A8-E34A-BCBA-976D0CA501C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D8808A-6273-F748-9C0A-5FE64059E51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{AE642143-4B0F-CF4A-8303-14EA69BAC89B}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="30240" windowHeight="17680" xr2:uid="{AE642143-4B0F-CF4A-8303-14EA69BAC89B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
     <t>Code and output in rendered document</t>
   </si>
   <si>
-    <t>PMAP 8551/4551 • Summer 2025</t>
+    <t>PMAP 8551/4551 • Fall 2025</t>
   </si>
 </sst>
 </file>
@@ -928,9 +928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550F01CB-66B6-2D48-9331-E85886CF5C6B}">
   <dimension ref="B2:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>